<commit_message>
updated retracted in fsm
</commit_message>
<xml_diff>
--- a/Master Sketch/Variables-Globals and Macros.xlsx
+++ b/Master Sketch/Variables-Globals and Macros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\Documents\Cybathlon\cybathlon\Master Sketch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7345A74A-A655-4B00-89C5-F07D6E996BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B36B977-FA1F-483D-B77D-6437642D1183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25830" yWindow="2595" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{2F9B3B66-C287-4F3D-8BCF-2301D49EF948}"/>
+    <workbookView xWindow="14250" yWindow="4260" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{2F9B3B66-C287-4F3D-8BCF-2301D49EF948}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -401,6 +401,39 @@
   </si>
   <si>
     <t>error for how close to 0 encoders are to be deemed "0"</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>fully_retracted</t>
+  </si>
+  <si>
+    <t>global variable for keeping track of if the leg is fully retracted</t>
+  </si>
+  <si>
+    <t>fully_extended</t>
+  </si>
+  <si>
+    <t>global variable for keeping track of if the leg is fully extended</t>
+  </si>
+  <si>
+    <t>retracted</t>
+  </si>
+  <si>
+    <t>global variable for keeping track of whether the leg has been retracted recently (reset to false when leg changes out of RETRACTED State)</t>
+  </si>
+  <si>
+    <t>RET_ANG</t>
+  </si>
+  <si>
+    <t>EXT_ANG</t>
+  </si>
+  <si>
+    <t>angle of fully retracted leg</t>
+  </si>
+  <si>
+    <t>angle of fully extended leg</t>
   </si>
 </sst>
 </file>
@@ -761,11 +794,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EC7646-CABC-4DEE-8A7F-AB4CA0776CF8}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,88 +837,88 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,10 +929,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,13 +940,13 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,13 +954,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,13 +968,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -952,37 +985,79 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -994,11 +1069,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BA4F2E-551D-4FA6-877D-AE48EA06A4EF}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,26 +1414,26 @@
         <v>97</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" t="s">
+        <v>132</v>
+      </c>
+    </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1366,10 +1441,10 @@
         <v>98</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1377,10 +1452,10 @@
         <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1388,10 +1463,10 @@
         <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1399,10 +1474,10 @@
         <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1410,10 +1485,10 @@
         <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1421,10 +1496,10 @@
         <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,10 +1507,10 @@
         <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1443,10 +1518,10 @@
         <v>98</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1454,10 +1529,10 @@
         <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,9 +1540,31 @@
         <v>98</v>
       </c>
       <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
         <v>110</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>